<commit_message>
add dictionary for excel home
</commit_message>
<xml_diff>
--- a/DKS-API/Resources/Template/TempP206DataByArticle.xlsx
+++ b/DKS-API/Resources/Template/TempP206DataByArticle.xlsx
@@ -169,7 +169,7 @@
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
     <numFmt numFmtId="177" formatCode="0_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -201,8 +201,14 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="20"/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -293,7 +299,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -612,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -638,7 +644,7 @@
     <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="11" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
@@ -696,7 +702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>